<commit_message>
Add Flow Sensor 2 Board
Incomplete
</commit_message>
<xml_diff>
--- a/Hardware/Electrical Components/Module - Power/BOM Power module.xlsx
+++ b/Hardware/Electrical Components/Module - Power/BOM Power module.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB15B3F-98BF-4507-8A03-EBACEF77D9B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB25B6B-378B-4918-B627-33FE192C8BD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Module" sheetId="1" r:id="rId1"/>
+    <sheet name="Mouser" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -18,7 +19,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="74">
   <si>
     <t>Name</t>
   </si>
@@ -209,6 +212,45 @@
   </si>
   <si>
     <t>Resistor 64K ohm 3.5mm</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>757-TC4S584FLF</t>
+  </si>
+  <si>
+    <t>621-1N4148W-F</t>
+  </si>
+  <si>
+    <t>594-K151J15C0GF5TH5</t>
+  </si>
+  <si>
+    <t>652-CR1206FX-2002ELF</t>
+  </si>
+  <si>
+    <t>595-TPIC6B595DWR</t>
+  </si>
+  <si>
+    <t>595-DRV8871DDAR</t>
+  </si>
+  <si>
+    <t>474-BOB-12009</t>
+  </si>
+  <si>
+    <t>80-C322C104K1R</t>
+  </si>
+  <si>
+    <t>594-SFR16S0006042FR5</t>
+  </si>
+  <si>
+    <t>647-UWT1C471MNL1S</t>
+  </si>
+  <si>
+    <t>651-1864286</t>
+  </si>
+  <si>
+    <t>80-C1206C104M5REAULR</t>
   </si>
 </sst>
 </file>
@@ -284,7 +326,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -314,6 +356,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -604,18 +651,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="8" max="8" width="16" style="9" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5546875" customWidth="1"/>
+    <col min="12" max="12" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -644,15 +691,15 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
       <c r="H3" s="9" t="s">
         <v>37</v>
       </c>
@@ -677,15 +724,15 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="20" t="s">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B4" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
       <c r="H4" s="9" t="s">
         <v>38</v>
       </c>
@@ -710,15 +757,15 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="20" t="s">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B5" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
       <c r="H5" s="9" t="s">
         <v>47</v>
       </c>
@@ -745,15 +792,15 @@
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="21" t="s">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B6" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
       <c r="H6" s="10" t="s">
         <v>39</v>
       </c>
@@ -778,15 +825,15 @@
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
     </row>
-    <row r="7" spans="2:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="22" t="s">
+    <row r="7" spans="2:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="19" t="s">
         <v>51</v>
       </c>
@@ -809,15 +856,15 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="21" t="s">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B8" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
       <c r="H8" s="10" t="s">
         <v>40</v>
       </c>
@@ -842,15 +889,15 @@
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B9" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
       <c r="H9" s="10" t="s">
         <v>41</v>
       </c>
@@ -877,15 +924,15 @@
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="21" t="s">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B10" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
       <c r="H10" s="10" t="s">
         <v>42</v>
       </c>
@@ -912,15 +959,15 @@
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="21" t="s">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B11" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
       <c r="H11" s="16" t="s">
         <v>57</v>
       </c>
@@ -945,15 +992,15 @@
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="s">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B12" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
       <c r="H12" s="18" t="s">
         <v>59</v>
       </c>
@@ -978,15 +1025,15 @@
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
     </row>
-    <row r="13" spans="2:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="22" t="s">
+    <row r="13" spans="2:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
       <c r="H13" s="11" t="s">
         <v>43</v>
       </c>
@@ -1010,15 +1057,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="20" t="s">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B14" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
       <c r="H14" s="13" t="s">
         <v>54</v>
       </c>
@@ -1045,15 +1092,15 @@
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="21" t="s">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B15" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
       <c r="H15" s="10" t="s">
         <v>44</v>
       </c>
@@ -1078,15 +1125,15 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="21" t="s">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B16" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
       <c r="H16" s="10" t="s">
         <v>45</v>
       </c>
@@ -1111,15 +1158,15 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="21" t="s">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B17" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
       <c r="H17" s="10" t="s">
         <v>46</v>
       </c>
@@ -1144,23 +1191,23 @@
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
       <c r="K19" t="s">
         <v>27</v>
       </c>
@@ -1170,15 +1217,15 @@
         <v>30.126999999999999</v>
       </c>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B20" s="21" t="s">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B20" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
       <c r="H20" s="6">
         <f>75.95/3</f>
         <v>25.316666666666666</v>
@@ -1191,23 +1238,23 @@
         <v>55.443666666666665</v>
       </c>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-    </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B32" s="20" t="s">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B32" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
       <c r="I32">
         <v>1</v>
       </c>
@@ -1228,13 +1275,13 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="21">
@@ -1281,4 +1328,570 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A861C2-3E4C-4EC3-9709-FFAD92322619}">
+  <dimension ref="B2:M20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B3" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="20">
+        <v>1</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L3" s="5">
+        <v>2.95</v>
+      </c>
+      <c r="M3" s="6">
+        <f t="shared" ref="M3:M15" si="0">I3*L3</f>
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20">
+        <v>1</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="20">
+        <v>10</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L5" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="M5" s="6">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="20">
+        <v>2</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="M6" s="6">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" s="19">
+        <v>4</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" s="5">
+        <v>0.52</v>
+      </c>
+      <c r="M7" s="6">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8" s="20">
+        <v>1</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" s="7">
+        <v>0.97</v>
+      </c>
+      <c r="M8" s="6">
+        <f t="shared" si="0"/>
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B9" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" s="20">
+        <v>2</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" s="7">
+        <v>0.44</v>
+      </c>
+      <c r="M9" s="6">
+        <f t="shared" si="0"/>
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B10" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="I10" s="20">
+        <v>2</v>
+      </c>
+      <c r="J10" s="8">
+        <v>1206</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L10" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="M10" s="6">
+        <f t="shared" si="0"/>
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="I11" s="20">
+        <v>24</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" s="7">
+        <v>0.161</v>
+      </c>
+      <c r="M11" s="6">
+        <f t="shared" si="0"/>
+        <v>3.8639999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" s="20">
+        <v>6</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L12" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="M12" s="6">
+        <f>I12*L12</f>
+        <v>0.89999999999999991</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B13" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13" s="20">
+        <v>33</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L13" s="7">
+        <v>0.151</v>
+      </c>
+      <c r="M13" s="6">
+        <f>I13*L13</f>
+        <v>4.9829999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B14" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14" s="20">
+        <v>2</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="L14" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="M14" s="6">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B15" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" s="20">
+        <v>2</v>
+      </c>
+      <c r="J15" s="8">
+        <v>1206</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L15" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="M15" s="6">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B16" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="I16" s="20">
+        <v>4</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L16" s="5">
+        <v>1.36</v>
+      </c>
+      <c r="M16" s="6">
+        <f>I16*L16</f>
+        <v>5.44</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B17" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="I17" s="20">
+        <v>2</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L17" s="5">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="M17" s="6">
+        <f>I17*L17</f>
+        <v>5.0199999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6">
+        <f>SUM(M3:M17)</f>
+        <v>29.637</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B20" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="6">
+        <f>75.95/3</f>
+        <v>25.316666666666666</v>
+      </c>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="L20" s="20"/>
+      <c r="M20" s="6">
+        <f>M19+H20</f>
+        <v>54.953666666666663</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="K8" r:id="rId1" xr:uid="{2EDFEFBB-F97E-41C3-BD6E-5F406FAF60A1}"/>
+    <hyperlink ref="K9" r:id="rId2" xr:uid="{2E60FF95-AA28-47B7-9BA9-DB59879FF379}"/>
+    <hyperlink ref="K10" r:id="rId3" xr:uid="{A8CB91B5-29BC-43D7-9B70-D3FB2388CAA0}"/>
+    <hyperlink ref="K16" r:id="rId4" xr:uid="{FC4C9F39-A864-4736-8B57-AA00FF7D6D03}"/>
+    <hyperlink ref="K3" r:id="rId5" xr:uid="{37287F72-7017-48EC-8E08-41A728F37DC7}"/>
+    <hyperlink ref="K17" r:id="rId6" xr:uid="{A8B02F69-FB8C-45C7-B0A7-C069073E037E}"/>
+    <hyperlink ref="K13" r:id="rId7" xr:uid="{D31EE695-52EF-4FBA-B31D-750ABAAEC927}"/>
+    <hyperlink ref="K5" r:id="rId8" xr:uid="{D88DE2C8-97FE-4966-8F27-E68B48C71F55}"/>
+    <hyperlink ref="K6" r:id="rId9" xr:uid="{EC0FCE91-138E-488F-9543-AA898FE6FC7E}"/>
+    <hyperlink ref="K15" r:id="rId10" xr:uid="{C319DCED-F22C-4607-95EA-B293289287CA}"/>
+    <hyperlink ref="K12" r:id="rId11" xr:uid="{B467B0D5-F31D-46FB-B007-5AAA9563E3A2}"/>
+    <hyperlink ref="K7" r:id="rId12" xr:uid="{0B9AC36D-26D2-4BE5-AC0E-A57DF0B5A87F}"/>
+    <hyperlink ref="K14" r:id="rId13" xr:uid="{1D852C78-A8C2-4439-B61C-FBD49F90A389}"/>
+    <hyperlink ref="K11" r:id="rId14" xr:uid="{1C505E69-99F8-4D33-81B6-8CBA81AC39DB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
+</worksheet>
 </file>
</xml_diff>